<commit_message>
+ Update physicists list to Optional 3-1
</commit_message>
<xml_diff>
--- a/school-book-physicists/physicists_list.xlsx
+++ b/school-book-physicists/physicists_list.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B9AF5A14-C2A7-46D6-AC8F-5001B6BE7BAA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{305FC5D3-0BD9-4DA4-AB3C-31624DBA782E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$55</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,10 +157,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>托勒玫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>列文虎克</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,6 +194,323 @@
   </si>
   <si>
     <t>托里拆利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>九年级上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>焦耳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瓦特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道尔顿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巴本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纽科门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安培</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伏特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欧姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昂内斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥斯特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法拉第</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>九年级下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摩斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麦克斯韦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>髙锟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝克勒尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皮埃尔·居里</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逝世</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玛丽·居里</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高中 必修1</t>
+  </si>
+  <si>
+    <t>高中 必修1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>达·芬奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沃森</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>克里克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈雷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱德华·洛伦兹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>威廉·汤姆生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>诺贝尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>德布罗意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莱布尼茨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李政道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨振宁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G.霍尔顿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普朗克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胡克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笛卡尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丁肇中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴健雄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J.韦伯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J.H.泰勒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密立根</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高中 必修2</t>
+  </si>
+  <si>
+    <t>托勒密</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基尔霍夫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉普拉斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第谷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>布鲁诺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰·柯西·亚当斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥本·勒维耶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰·格弗里恩·伽勒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冯·劳厄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>霍金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F.W.贝塞尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戴维</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塞贝克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尤里乌斯·冯·迈尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亥姆霍兹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选修 3-1</t>
+  </si>
+  <si>
+    <t>选修 3-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>温伯格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格拉肖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨拉姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰·施瓦茨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迈克尔·格林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱德华·威滕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰勒斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>威廉·吉尔伯特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>库仑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范德格拉夫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>埃米利奥·塞格雷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欧文·张伯伦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>托马斯·杨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特斯拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亨德里克·洛伦兹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E.H.霍尔</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,22 +851,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,8 +887,17 @@
       <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -581,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -592,7 +919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -603,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -614,7 +941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -625,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -636,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -647,7 +974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -658,7 +985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -669,7 +996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -680,7 +1007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -691,7 +1018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -702,7 +1029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -713,7 +1040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -724,7 +1051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -847,7 +1174,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>22</v>
@@ -858,7 +1185,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>22</v>
@@ -869,7 +1196,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -880,7 +1207,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>22</v>
@@ -891,7 +1218,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>22</v>
@@ -902,7 +1229,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>22</v>
@@ -913,7 +1240,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>22</v>
@@ -924,7 +1251,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>22</v>
@@ -935,7 +1262,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>22</v>
@@ -946,7 +1273,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>22</v>
@@ -957,7 +1284,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>22</v>
@@ -966,7 +1293,767 @@
         <v>36</v>
       </c>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>102</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>104</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>118</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>119</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>120</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>122</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F106">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I55" xr:uid="{10DE199A-405D-4677-A6DA-BB17E1C7D46B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>